<commit_message>
BOM links activated in the pdf
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM v1.1.0.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM v1.1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="604" documentId="11_BB46956AE7341EA83D7747123DA4EA88538076BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF153A3-80A5-4976-B88D-EB2BD62778F6}"/>
+  <xr:revisionPtr revIDLastSave="628" documentId="11_BB46956AE7341EA83D7747123DA4EA88538076BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF2E1F17-4123-4526-B544-A3259973B9AA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valkyrie Stage-I" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="332">
   <si>
     <t>Develompment Team Members</t>
   </si>
@@ -898,9 +898,6 @@
   </si>
   <si>
     <t>Hotend</t>
-  </si>
-  <si>
-    <t>Bondtech</t>
   </si>
   <si>
     <t>Motionparts</t>
@@ -1382,9 +1379,6 @@
     <t>1x Size: 2M ID 4MM OD 6MM</t>
   </si>
   <si>
-    <t>Color: 369 mm</t>
-  </si>
-  <si>
     <t>Antfox Store</t>
   </si>
   <si>
@@ -1451,9 +1445,6 @@
     <t>FABREEKO</t>
   </si>
   <si>
-    <t>HoneyBadger Stainless Steel Rails</t>
-  </si>
-  <si>
     <t>HoneyBadger Frame &amp; Bracket Parts</t>
   </si>
   <si>
@@ -1511,13 +1502,67 @@
     <t>2xMGN12H/400mm Medium PL</t>
   </si>
   <si>
-    <t>MGN 12h - Z Axis Medium PL</t>
-  </si>
-  <si>
-    <t>MGN 12h - Y Axis Medium PL</t>
-  </si>
-  <si>
-    <t>MGN 9h - X Axis Medium PL</t>
+    <r>
+      <t xml:space="preserve">MGN 12h-Z Axis. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NB! See note</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGN 12h-Y Axis. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NB! See note</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MGN 9h-Z Axis. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NB! See note</t>
+    </r>
+  </si>
+  <si>
+    <t>HoneyBadger High Temp Rails</t>
+  </si>
+  <si>
+    <t>3xMGN 12H/350mm. NB! See note</t>
+  </si>
+  <si>
+    <t>2xMGN12H/400mm. NB! See note</t>
+  </si>
+  <si>
+    <t>1xMGN9H/400mm. NB! Seee note</t>
+  </si>
+  <si>
+    <t>BTT</t>
+  </si>
+  <si>
+    <t>Color: 339 mm</t>
   </si>
 </sst>
 </file>
@@ -2915,6 +2960,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:L59" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
   <tableColumns count="12">
@@ -3179,9 +3228,9 @@
   </sheetPr>
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:K13"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3202,7 +3251,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" hidden="1" thickBot="1">
       <c r="A1" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B1" s="115"/>
       <c r="C1" s="115"/>
@@ -3221,7 +3270,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>5</v>
@@ -3233,7 +3282,7 @@
       <c r="H2" s="44"/>
       <c r="I2" s="45">
         <f>I60</f>
-        <v>1862.6400000000003</v>
+        <v>2028.6400000000003</v>
       </c>
       <c r="J2" s="43"/>
       <c r="K2" s="50"/>
@@ -3294,7 +3343,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="21">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="F4" s="22">
         <v>1</v>
@@ -3308,8 +3357,8 @@
       <c r="I4" s="38">
         <v>8</v>
       </c>
-      <c r="J4" s="57" t="s">
-        <v>283</v>
+      <c r="J4" s="26" t="s">
+        <v>331</v>
       </c>
       <c r="K4" s="28" t="s">
         <v>24</v>
@@ -3509,14 +3558,14 @@
         <v>20</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K9" s="27" t="s">
         <v>24</v>
       </c>
       <c r="L9" s="69"/>
       <c r="M9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N9" s="86"/>
     </row>
@@ -3531,7 +3580,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F10" s="9">
         <v>4</v>
@@ -3547,14 +3596,14 @@
         <v>40</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K10" s="27" t="s">
         <v>24</v>
       </c>
       <c r="L10" s="71"/>
       <c r="M10" s="87" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N10" s="86"/>
     </row>
@@ -3563,13 +3612,13 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" t="s">
-        <v>326</v>
+        <v>149</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="E11">
         <v>350</v>
@@ -3588,14 +3637,14 @@
         <v>55.5</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L11" s="72"/>
       <c r="M11" s="87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="N11" s="86"/>
     </row>
@@ -3604,13 +3653,13 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>327</v>
+        <v>149</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="E12">
         <v>400</v>
@@ -3629,14 +3678,14 @@
         <v>39</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L12" s="72"/>
       <c r="M12" s="87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N12" s="86"/>
     </row>
@@ -3645,13 +3694,13 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" t="s">
-        <v>328</v>
+        <v>149</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="E13">
         <v>400</v>
@@ -3670,10 +3719,10 @@
         <v>17.5</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L13" s="72"/>
       <c r="M13" s="2"/>
@@ -3690,14 +3739,14 @@
         <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
       <c r="H14" s="9"/>
       <c r="I14" s="80">
         <f>G18+G19</f>
-        <v>374</v>
+        <v>535</v>
       </c>
       <c r="J14" s="55"/>
       <c r="K14" s="27"/>
@@ -3716,7 +3765,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="107" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E15" s="107"/>
       <c r="F15" s="108"/>
@@ -3725,11 +3774,11 @@
       <c r="I15" s="110"/>
       <c r="J15" s="111"/>
       <c r="K15" s="112" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="L15" s="73"/>
       <c r="M15" s="116" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="N15" s="117"/>
     </row>
@@ -3744,7 +3793,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="92">
@@ -3759,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="69" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K16" s="102" t="s">
         <v>43</v>
@@ -3779,7 +3828,7 @@
         <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="92">
@@ -3794,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="69" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K17" s="102" t="s">
         <v>43</v>
@@ -3814,7 +3863,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="95" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E18" s="95"/>
       <c r="F18" s="96">
@@ -3829,10 +3878,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="68" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="K18" s="105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L18" s="69"/>
       <c r="M18" s="116"/>
@@ -3843,20 +3892,20 @@
         <v>46</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="99" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E19" s="99"/>
       <c r="F19" s="100">
         <v>1</v>
       </c>
       <c r="G19" s="101">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="H19" s="100"/>
       <c r="I19" s="104">
@@ -3864,10 +3913,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="113" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K19" s="103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L19" s="69"/>
       <c r="M19" s="116"/>
@@ -3884,7 +3933,7 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E20">
         <v>410</v>
@@ -3903,7 +3952,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>38</v>
@@ -3923,7 +3972,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E21">
         <v>230</v>
@@ -3942,7 +3991,7 @@
         <v>35</v>
       </c>
       <c r="J21" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K21" s="41" t="s">
         <v>38</v>
@@ -3987,7 +4036,7 @@
       </c>
       <c r="L22" s="74"/>
       <c r="M22" s="116" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="N22" s="117"/>
     </row>
@@ -4002,7 +4051,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23">
         <v>330</v>
@@ -4021,13 +4070,13 @@
         <v>46</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="L23" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M23" s="116"/>
       <c r="N23" s="117"/>
@@ -4102,7 +4151,7 @@
       </c>
       <c r="L25" s="74"/>
       <c r="M25" s="116" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N25" s="117"/>
     </row>
@@ -4117,7 +4166,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F26" s="9">
         <v>1</v>
@@ -4133,13 +4182,13 @@
         <v>145</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>111</v>
       </c>
       <c r="L26" s="72" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M26" s="116"/>
       <c r="N26" s="117"/>
@@ -4227,7 +4276,7 @@
         <v>120</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E29">
         <v>300</v>
@@ -4246,13 +4295,13 @@
         <v>78.39</v>
       </c>
       <c r="J29" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L29" s="72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M29" s="89"/>
       <c r="N29" s="86"/>
@@ -4284,10 +4333,10 @@
         <v>52</v>
       </c>
       <c r="J30" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L30" s="72" t="s">
         <v>122</v>
@@ -4306,7 +4355,7 @@
         <v>124</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F31" s="9">
         <v>1</v>
@@ -4322,7 +4371,7 @@
         <v>3</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K31" s="12" t="s">
         <v>125</v>
@@ -4339,10 +4388,10 @@
         <v>109</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D32" t="s">
         <v>189</v>
-      </c>
-      <c r="D32" t="s">
-        <v>190</v>
       </c>
       <c r="F32" s="9">
         <v>1</v>
@@ -4358,13 +4407,13 @@
         <v>2</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K32" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L32" s="72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M32" s="89"/>
       <c r="N32" s="86"/>
@@ -4380,7 +4429,7 @@
         <v>127</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F33" s="9">
         <v>1</v>
@@ -4396,10 +4445,10 @@
         <v>40</v>
       </c>
       <c r="J33" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K33" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L33" s="74"/>
       <c r="M33" s="89"/>
@@ -4413,10 +4462,10 @@
         <v>126</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D34" t="s">
         <v>218</v>
-      </c>
-      <c r="D34" t="s">
-        <v>219</v>
       </c>
       <c r="F34" s="9">
         <v>1</v>
@@ -4432,7 +4481,7 @@
         <v>13.5</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K34" s="41" t="s">
         <v>119</v>
@@ -4452,26 +4501,26 @@
         <v>126</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F35" s="9">
         <v>1</v>
       </c>
       <c r="G35" s="10">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H35" s="9">
         <v>1</v>
       </c>
       <c r="I35" s="39">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J35" s="47" t="s">
-        <v>321</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>128</v>
+        <v>318</v>
+      </c>
+      <c r="K35" s="81" t="s">
+        <v>330</v>
       </c>
       <c r="L35" s="74"/>
       <c r="M35" s="89"/>
@@ -4488,7 +4537,7 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F36" s="9">
         <v>1</v>
@@ -4504,10 +4553,10 @@
         <v>3.75</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L36" s="75"/>
       <c r="M36" s="89"/>
@@ -4524,7 +4573,7 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F37" s="9">
         <v>2</v>
@@ -4540,10 +4589,10 @@
         <v>10</v>
       </c>
       <c r="J37" s="47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L37" s="75"/>
       <c r="M37" s="89"/>
@@ -4626,13 +4675,13 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" t="s">
         <v>130</v>
-      </c>
-      <c r="D40" t="s">
-        <v>131</v>
       </c>
       <c r="F40" s="9">
         <v>8</v>
@@ -4648,7 +4697,7 @@
         <v>59</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>119</v>
@@ -4662,13 +4711,13 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
         <v>133</v>
-      </c>
-      <c r="D41" t="s">
-        <v>134</v>
       </c>
       <c r="F41" s="9">
         <v>10</v>
@@ -4684,10 +4733,10 @@
         <v>41</v>
       </c>
       <c r="J41" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="K41" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="L41" s="74"/>
       <c r="M41" s="89"/>
@@ -4698,13 +4747,13 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F42" s="9">
         <v>5</v>
@@ -4720,10 +4769,10 @@
         <v>30</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L42" s="74"/>
       <c r="M42" s="89"/>
@@ -4734,13 +4783,13 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" t="s">
         <v>139</v>
-      </c>
-      <c r="D43" t="s">
-        <v>140</v>
       </c>
       <c r="F43" s="9">
         <v>5</v>
@@ -4756,10 +4805,10 @@
         <v>20</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L43" s="74"/>
       <c r="M43" s="89"/>
@@ -4770,13 +4819,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C44" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" t="s">
         <v>142</v>
-      </c>
-      <c r="D44" t="s">
-        <v>143</v>
       </c>
       <c r="E44">
         <v>200</v>
@@ -4795,10 +4844,10 @@
         <v>48</v>
       </c>
       <c r="J44" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="K44" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="L44" s="74"/>
       <c r="M44" s="89"/>
@@ -4809,13 +4858,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" t="s">
         <v>146</v>
-      </c>
-      <c r="D45" t="s">
-        <v>147</v>
       </c>
       <c r="F45" s="9">
         <v>5</v>
@@ -4831,10 +4880,10 @@
         <v>72.5</v>
       </c>
       <c r="J45" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="K45" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="L45" s="75"/>
       <c r="M45" s="89"/>
@@ -4842,16 +4891,16 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" t="s">
         <v>153</v>
       </c>
-      <c r="B46" t="s">
-        <v>154</v>
-      </c>
       <c r="C46" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F46" s="9">
         <v>5</v>
@@ -4867,10 +4916,10 @@
         <v>60</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K46" s="82" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L46" s="76"/>
       <c r="M46" s="89"/>
@@ -4878,16 +4927,16 @@
     </row>
     <row r="47" spans="1:14" ht="14.45" customHeight="1">
       <c r="A47" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>156</v>
-      </c>
       <c r="D47" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F47" s="9">
         <v>5</v>
@@ -4903,10 +4952,10 @@
         <v>125</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K47" s="82" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L47" s="76"/>
       <c r="M47" s="89"/>
@@ -4914,16 +4963,16 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C48" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>211</v>
       </c>
       <c r="E48">
         <v>300</v>
@@ -4942,10 +4991,10 @@
         <v>50</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L48" s="75"/>
       <c r="M48" s="89"/>
@@ -4953,16 +5002,16 @@
     </row>
     <row r="49" spans="1:14" ht="14.45" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
         <v>109</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D49" t="s">
         <v>277</v>
-      </c>
-      <c r="D49" t="s">
-        <v>278</v>
       </c>
       <c r="F49" s="9">
         <v>5</v>
@@ -4978,10 +5027,10 @@
         <v>16.149999999999999</v>
       </c>
       <c r="J49" s="47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L49" s="75"/>
       <c r="M49" s="89"/>
@@ -4989,16 +5038,16 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
         <v>109</v>
       </c>
       <c r="C50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
         <v>166</v>
-      </c>
-      <c r="D50" t="s">
-        <v>167</v>
       </c>
       <c r="F50" s="9">
         <v>1</v>
@@ -5014,10 +5063,10 @@
         <v>3</v>
       </c>
       <c r="J50" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="K50" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="L50" s="75"/>
       <c r="M50" s="89"/>
@@ -5025,16 +5074,16 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B51" t="s">
         <v>109</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F51" s="9">
         <v>2</v>
@@ -5050,10 +5099,10 @@
         <v>24</v>
       </c>
       <c r="J51" s="114" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L51" s="75"/>
       <c r="M51" s="89"/>
@@ -5061,7 +5110,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
         <v>109</v>
@@ -5070,7 +5119,7 @@
         <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F52" s="9">
         <v>1</v>
@@ -5086,10 +5135,10 @@
         <v>12</v>
       </c>
       <c r="J52" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="89"/>
@@ -5097,7 +5146,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>109</v>
@@ -5106,7 +5155,7 @@
         <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F53" s="9">
         <v>1</v>
@@ -5123,10 +5172,10 @@
         <v>3.96</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="89"/>
@@ -5134,16 +5183,16 @@
     </row>
     <row r="54" spans="1:14" ht="14.45" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="D54" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F54" s="9">
         <v>1</v>
@@ -5159,10 +5208,10 @@
         <v>3.72</v>
       </c>
       <c r="J54" s="47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K54" s="81" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L54" s="75"/>
       <c r="M54" s="89"/>
@@ -5170,16 +5219,16 @@
     </row>
     <row r="55" spans="1:14" ht="14.45" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F55" s="9">
         <v>1</v>
@@ -5195,10 +5244,10 @@
         <v>4</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L55" s="75"/>
       <c r="M55" s="89"/>
@@ -5206,16 +5255,16 @@
     </row>
     <row r="56" spans="1:14" ht="14.45" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F56" s="9">
         <v>1</v>
@@ -5231,10 +5280,10 @@
         <v>3</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L56" s="75"/>
       <c r="M56" s="89"/>
@@ -5242,16 +5291,16 @@
     </row>
     <row r="57" spans="1:14" ht="14.45" customHeight="1">
       <c r="A57" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D57" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F57" s="9">
         <v>1</v>
@@ -5267,10 +5316,10 @@
         <v>3</v>
       </c>
       <c r="J57" s="47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L57" s="75"/>
       <c r="M57" s="89"/>
@@ -5278,16 +5327,16 @@
     </row>
     <row r="58" spans="1:14" ht="14.45" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="D58" t="s">
         <v>195</v>
-      </c>
-      <c r="D58" t="s">
-        <v>196</v>
       </c>
       <c r="F58" s="9">
         <v>1</v>
@@ -5303,10 +5352,10 @@
         <v>21.5</v>
       </c>
       <c r="J58" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L58" s="77"/>
       <c r="M58" s="89"/>
@@ -5318,10 +5367,10 @@
         <v>65</v>
       </c>
       <c r="C59" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D59" s="60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E59" s="62"/>
       <c r="F59" s="63"/>
@@ -5345,7 +5394,7 @@
         <v>4</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D60" s="43" t="s">
         <v>5</v>
@@ -5356,7 +5405,7 @@
       <c r="H60" s="44"/>
       <c r="I60" s="45">
         <f>SUM(I20:I59)+I14</f>
-        <v>1862.6400000000003</v>
+        <v>2028.6400000000003</v>
       </c>
       <c r="J60" s="43"/>
       <c r="K60" s="50"/>
@@ -5417,7 +5466,7 @@
     <hyperlink ref="J36" r:id="rId42" xr:uid="{6B0C3554-C92C-477C-968B-C3A56DEE5BB2}"/>
     <hyperlink ref="J37" r:id="rId43" xr:uid="{230B31B2-E3E9-4D33-8792-EA389633978B}"/>
     <hyperlink ref="J21" r:id="rId44" xr:uid="{AE44EAD7-69DD-4806-9E2F-C1401214B95A}"/>
-    <hyperlink ref="J4" r:id="rId45" xr:uid="{DEB61E4F-1486-491A-838D-61337A0DB5B3}"/>
+    <hyperlink ref="J4" r:id="rId45" display="Color: 369 mm" xr:uid="{DEB61E4F-1486-491A-838D-61337A0DB5B3}"/>
     <hyperlink ref="J5" r:id="rId46" xr:uid="{B0B2353F-D76B-49D2-92E2-924AA7C3940B}"/>
     <hyperlink ref="J6" r:id="rId47" xr:uid="{A49E22B6-E552-4BE6-8729-184F520A838F}"/>
     <hyperlink ref="J7" r:id="rId48" xr:uid="{47004657-0518-4245-B471-B34B5125E399}"/>
@@ -5476,7 +5525,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" thickBot="1">
       <c r="A1" s="115" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="115"/>
       <c r="C1" s="115"/>
@@ -5562,10 +5611,10 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="s">
         <v>170</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -5582,10 +5631,10 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="G4" s="48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="52"/>
@@ -5652,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>50</v>
@@ -5669,7 +5718,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" s="9">
         <v>6</v>
@@ -5686,7 +5735,7 @@
         <v>0.49</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>50</v>
@@ -5705,7 +5754,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C8" s="9">
         <v>31</v>
@@ -5721,23 +5770,23 @@
         <v>0.74</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J8" s="51"/>
       <c r="L8" s="86"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="9">
         <v>8</v>
@@ -5752,7 +5801,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>50</v>
@@ -5762,7 +5811,7 @@
       </c>
       <c r="J9" s="51"/>
       <c r="K9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L9" s="86"/>
     </row>
@@ -5797,7 +5846,7 @@
         <v>7380</v>
       </c>
       <c r="K10" s="87" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L10" s="86"/>
     </row>
@@ -5806,7 +5855,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -5821,7 +5870,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H11" s="41" t="s">
         <v>50</v>
@@ -5833,7 +5882,7 @@
         <v>10642</v>
       </c>
       <c r="K11" s="87" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L11" s="86"/>
     </row>
@@ -5868,7 +5917,7 @@
       </c>
       <c r="J12" s="52"/>
       <c r="K12" s="87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L12" s="86"/>
     </row>
@@ -5910,7 +5959,7 @@
         <v>70</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C14">
         <v>29</v>
@@ -5925,7 +5974,7 @@
         <v>1.07</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H14" s="41" t="s">
         <v>50</v>
@@ -5970,7 +6019,7 @@
         <v>7380</v>
       </c>
       <c r="K15" s="116" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L15" s="117"/>
     </row>
@@ -5979,7 +6028,7 @@
         <v>70</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -5995,7 +6044,7 @@
         <v>1.5</v>
       </c>
       <c r="G16" s="47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>50</v>
@@ -6009,10 +6058,10 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" t="s">
         <v>175</v>
-      </c>
-      <c r="B17" t="s">
-        <v>176</v>
       </c>
       <c r="C17" s="9">
         <v>4</v>
@@ -6029,7 +6078,7 @@
         <v>3.27</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>50</v>
@@ -6041,10 +6090,10 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="9">
         <v>4</v>
@@ -6061,7 +6110,7 @@
         <v>2.57</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>50</v>
@@ -6069,7 +6118,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="51"/>
       <c r="K18" s="116" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L18" s="117"/>
     </row>
@@ -6094,7 +6143,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>79</v>
@@ -6109,7 +6158,7 @@
         <v>70</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -6125,7 +6174,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>79</v>
@@ -6168,7 +6217,7 @@
         <v>4032</v>
       </c>
       <c r="K21" s="116" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L21" s="117"/>
     </row>
@@ -6177,7 +6226,7 @@
         <v>66</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22">
         <v>9</v>
@@ -6317,7 +6366,7 @@
         <v>70</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -6333,7 +6382,7 @@
         <v>3.28</v>
       </c>
       <c r="G26" s="47" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>50</v>
@@ -6451,7 +6500,7 @@
         <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30">
         <v>72</v>
@@ -6479,10 +6528,10 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -6499,10 +6548,10 @@
         <v>3.62</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="51"/>
@@ -6615,7 +6664,7 @@
         <v>70</v>
       </c>
       <c r="B35" s="56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -6630,7 +6679,7 @@
         <v>1.64</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>79</v>
@@ -6680,7 +6729,7 @@
         <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C37">
         <v>15</v>
@@ -6696,7 +6745,7 @@
         <v>6.08</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>50</v>
@@ -6729,10 +6778,10 @@
         <v>16</v>
       </c>
       <c r="G38" s="47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I38" s="15"/>
       <c r="J38" s="51"/>
@@ -6744,7 +6793,7 @@
         <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C39" s="9">
         <v>1</v>
@@ -6759,10 +6808,10 @@
         <v>9.5</v>
       </c>
       <c r="G39" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="H39" s="41" t="s">
         <v>253</v>
-      </c>
-      <c r="H39" s="41" t="s">
-        <v>254</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="51"/>
@@ -6774,7 +6823,7 @@
         <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -6790,7 +6839,7 @@
         <v>4.5</v>
       </c>
       <c r="G40" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>60</v>
@@ -6805,7 +6854,7 @@
         <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C41" s="9">
         <v>6</v>
@@ -6814,16 +6863,16 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F41" s="39">
         <v>9.1999999999999993</v>
       </c>
       <c r="G41" s="47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="51"/>
@@ -6866,7 +6915,7 @@
         <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -6882,10 +6931,10 @@
         <v>24</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="52"/>
@@ -6897,7 +6946,7 @@
         <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -6914,10 +6963,10 @@
         <v>5.01</v>
       </c>
       <c r="G44" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="H44" s="12" t="s">
         <v>162</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>163</v>
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="52"/>
@@ -6926,10 +6975,10 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" t="s">
         <v>173</v>
-      </c>
-      <c r="B45" t="s">
-        <v>174</v>
       </c>
       <c r="C45" s="9">
         <v>1</v>
@@ -6946,10 +6995,10 @@
         <v>1.72</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="51"/>
@@ -7058,7 +7107,7 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
@@ -7081,7 +7130,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27">
       <c r="A1" s="115" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B1" s="115"/>
       <c r="C1" s="115"/>
@@ -7102,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -7114,7 +7163,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -7125,7 +7174,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -7135,7 +7184,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -7145,7 +7194,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>5</v>
@@ -7156,7 +7205,7 @@
       <c r="H6" s="44"/>
       <c r="I6" s="45">
         <f>I49</f>
-        <v>1462.31</v>
+        <v>1628.31</v>
       </c>
       <c r="J6" s="43"/>
       <c r="K6" s="50"/>
@@ -7214,7 +7263,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="21">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="F8" s="22">
         <v>1</v>
@@ -7229,7 +7278,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
       <c r="K8" s="28" t="s">
         <v>24</v>
@@ -7412,7 +7461,7 @@
         <v>25</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K13" s="27" t="s">
         <v>24</v>
@@ -7430,7 +7479,7 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F14" s="9">
         <v>4</v>
@@ -7446,7 +7495,7 @@
         <v>40</v>
       </c>
       <c r="J14" s="55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>24</v>
@@ -7458,13 +7507,13 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" t="s">
-        <v>326</v>
+        <v>149</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="E15">
         <v>350</v>
@@ -7483,10 +7532,10 @@
         <v>55.5</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L15" s="72"/>
     </row>
@@ -7495,13 +7544,13 @@
         <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" t="s">
-        <v>327</v>
+        <v>149</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="E16">
         <v>400</v>
@@ -7520,10 +7569,10 @@
         <v>39</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="K16" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L16" s="72"/>
     </row>
@@ -7532,13 +7581,13 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" t="s">
-        <v>328</v>
+        <v>149</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="E17">
         <v>400</v>
@@ -7557,10 +7606,10 @@
         <v>17.5</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L17" s="72"/>
       <c r="M17" s="2"/>
@@ -7576,14 +7625,14 @@
         <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
       <c r="H18" s="9"/>
       <c r="I18" s="80">
         <f>G22+G23</f>
-        <v>374</v>
+        <v>535</v>
       </c>
       <c r="J18" s="55"/>
       <c r="K18" s="27"/>
@@ -7600,7 +7649,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="107" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E19" s="107"/>
       <c r="F19" s="108"/>
@@ -7609,7 +7658,7 @@
       <c r="I19" s="110"/>
       <c r="J19" s="111"/>
       <c r="K19" s="112" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="L19" s="73"/>
     </row>
@@ -7624,7 +7673,7 @@
         <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="92">
@@ -7639,7 +7688,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="69" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K20" s="102" t="s">
         <v>43</v>
@@ -7657,7 +7706,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="92">
@@ -7672,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="69" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K21" s="102" t="s">
         <v>43</v>
@@ -7690,7 +7739,7 @@
         <v>35</v>
       </c>
       <c r="D22" s="95" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E22" s="95"/>
       <c r="F22" s="96">
@@ -7705,10 +7754,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="68" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="K22" s="105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L22" s="69"/>
     </row>
@@ -7717,20 +7766,20 @@
         <v>46</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="99" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E23" s="99"/>
       <c r="F23" s="100">
         <v>1</v>
       </c>
       <c r="G23" s="101">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="H23" s="100"/>
       <c r="I23" s="104">
@@ -7738,10 +7787,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="113" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K23" s="103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L23" s="69"/>
     </row>
@@ -7775,7 +7824,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>38</v>
@@ -7829,7 +7878,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E26">
         <v>330</v>
@@ -7848,13 +7897,13 @@
         <v>46</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>45</v>
       </c>
       <c r="L26" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -7936,7 +7985,7 @@
         <v>110</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F29" s="9">
         <v>1</v>
@@ -7952,13 +8001,13 @@
         <v>145</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>111</v>
       </c>
       <c r="L29" s="72" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -8040,7 +8089,7 @@
         <v>120</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E32">
         <v>300</v>
@@ -8059,13 +8108,13 @@
         <v>78.39</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L32" s="72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -8095,10 +8144,10 @@
         <v>26</v>
       </c>
       <c r="J33" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L33" s="72" t="s">
         <v>122</v>
@@ -8115,7 +8164,7 @@
         <v>124</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F34" s="9">
         <v>1</v>
@@ -8131,7 +8180,7 @@
         <v>3</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>125</v>
@@ -8146,10 +8195,10 @@
         <v>109</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" t="s">
         <v>189</v>
-      </c>
-      <c r="D35" t="s">
-        <v>190</v>
       </c>
       <c r="F35" s="9">
         <v>1</v>
@@ -8165,13 +8214,13 @@
         <v>2</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K35" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L35" s="72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -8185,7 +8234,7 @@
         <v>127</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F36" s="9">
         <v>1</v>
@@ -8201,10 +8250,10 @@
         <v>40</v>
       </c>
       <c r="J36" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K36" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L36" s="74"/>
     </row>
@@ -8216,10 +8265,10 @@
         <v>126</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" t="s">
         <v>218</v>
-      </c>
-      <c r="D37" t="s">
-        <v>219</v>
       </c>
       <c r="F37" s="9">
         <v>1</v>
@@ -8235,7 +8284,7 @@
         <v>13.5</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K37" s="41" t="s">
         <v>119</v>
@@ -8253,26 +8302,26 @@
         <v>126</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F38" s="9">
         <v>1</v>
       </c>
       <c r="G38" s="10">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H38" s="9">
         <v>1</v>
       </c>
       <c r="I38" s="39">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J38" s="47" t="s">
-        <v>321</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>128</v>
+        <v>318</v>
+      </c>
+      <c r="K38" s="81" t="s">
+        <v>330</v>
       </c>
       <c r="L38" s="74"/>
       <c r="M38" s="89"/>
@@ -8288,7 +8337,7 @@
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F39" s="9">
         <v>1</v>
@@ -8304,10 +8353,10 @@
         <v>3.75</v>
       </c>
       <c r="J39" s="47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L39" s="75"/>
     </row>
@@ -8384,13 +8433,13 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" t="s">
         <v>130</v>
-      </c>
-      <c r="D42" t="s">
-        <v>131</v>
       </c>
       <c r="F42" s="9">
         <v>8</v>
@@ -8406,7 +8455,7 @@
         <v>59</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>119</v>
@@ -8418,13 +8467,13 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
         <v>133</v>
-      </c>
-      <c r="D43" t="s">
-        <v>134</v>
       </c>
       <c r="F43" s="9">
         <v>10</v>
@@ -8440,10 +8489,10 @@
         <v>41</v>
       </c>
       <c r="J43" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="K43" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="L43" s="74"/>
     </row>
@@ -8452,13 +8501,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F44" s="9">
         <v>5</v>
@@ -8474,10 +8523,10 @@
         <v>30</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L44" s="74"/>
     </row>
@@ -8486,13 +8535,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" t="s">
         <v>139</v>
-      </c>
-      <c r="D45" t="s">
-        <v>140</v>
       </c>
       <c r="F45" s="9">
         <v>5</v>
@@ -8508,10 +8557,10 @@
         <v>20</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L45" s="74"/>
     </row>
@@ -8520,13 +8569,13 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" t="s">
         <v>142</v>
-      </c>
-      <c r="D46" t="s">
-        <v>143</v>
       </c>
       <c r="E46">
         <v>200</v>
@@ -8545,10 +8594,10 @@
         <v>48</v>
       </c>
       <c r="J46" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="K46" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="L46" s="74"/>
     </row>
@@ -8557,13 +8606,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" t="s">
         <v>146</v>
-      </c>
-      <c r="D47" t="s">
-        <v>147</v>
       </c>
       <c r="F47" s="9">
         <v>5</v>
@@ -8579,10 +8628,10 @@
         <v>72.5</v>
       </c>
       <c r="J47" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="K47" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="L47" s="75"/>
     </row>
@@ -8592,10 +8641,10 @@
         <v>65</v>
       </c>
       <c r="C48" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D48" s="60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E48" s="62"/>
       <c r="F48" s="63"/>
@@ -8617,7 +8666,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>5</v>
@@ -8628,7 +8677,7 @@
       <c r="H49" s="44"/>
       <c r="I49" s="45">
         <f>SUM(I24:I48)+I18</f>
-        <v>1462.31</v>
+        <v>1628.31</v>
       </c>
       <c r="J49" s="43"/>
       <c r="K49" s="50"/>
@@ -8670,7 +8719,7 @@
     <hyperlink ref="E3" r:id="rId29" xr:uid="{8D7BE965-D64F-4EF6-AB85-6D60325E0F14}"/>
     <hyperlink ref="E4" r:id="rId30" xr:uid="{1AB1BA1F-E652-4A59-AFD9-CF100F7A0675}"/>
     <hyperlink ref="E5" r:id="rId31" xr:uid="{E1E6DD43-4F3E-40D4-869F-6509B89AF289}"/>
-    <hyperlink ref="J8" r:id="rId32" xr:uid="{EC02321E-B7C3-4FC1-B874-04DFA25238EB}"/>
+    <hyperlink ref="J8" r:id="rId32" display="Color: 369 mm" xr:uid="{EC02321E-B7C3-4FC1-B874-04DFA25238EB}"/>
     <hyperlink ref="J9" r:id="rId33" xr:uid="{75B54B15-A33C-4E87-8110-F508CB5C1277}"/>
     <hyperlink ref="J10" r:id="rId34" xr:uid="{83361321-C27C-4029-97C6-080CDFE55588}"/>
     <hyperlink ref="J11" r:id="rId35" xr:uid="{3ED6FC78-17EA-44FD-B607-926496CA6227}"/>
@@ -8687,7 +8736,7 @@
     <hyperlink ref="J17" r:id="rId46" display="3xGL: 350 - C: MGN12 H" xr:uid="{85E708C4-24F3-4615-975D-E526035BAA0A}"/>
   </hyperlinks>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId47"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId47"/>
   <drawing r:id="rId48"/>
   <legacyDrawing r:id="rId49"/>
   <tableParts count="1">

</xml_diff>